<commit_message>
Melhoramento do codigo Aperfeiçoamento Screenshot
</commit_message>
<xml_diff>
--- a/src/main/java/br/com/rsinet/hub_tdd/cadastro/cadastro.xlsx
+++ b/src/main/java/br/com/rsinet/hub_tdd/cadastro/cadastro.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rodrigo.vilhena\Documents\AvaliacaoTDD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DDC4883-EA50-4028-A4C4-4CA72FBCF36B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74A6D8DE-561E-4526-A0AE-E2EE3A74EA5A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" activeTab="1" xr2:uid="{335E1E31-5428-4F3C-9976-AAC697D51952}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{335E1E31-5428-4F3C-9976-AAC697D51952}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>Usuario</t>
   </si>
@@ -100,23 +100,23 @@
     <t>t123123</t>
   </si>
   <si>
-    <t>RodrigoVilhena</t>
-  </si>
-  <si>
-    <t>rodrigovilhenateste@rstinet.com.br</t>
-  </si>
-  <si>
     <t>Produto busca</t>
   </si>
   <si>
     <t>HP Z4000 WIRELESS MOUSE</t>
+  </si>
+  <si>
+    <t>RodrigoVil55</t>
+  </si>
+  <si>
+    <t>rodrigovilnateste@rstinet.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,6 +127,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF2A2A2A"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -297,10 +305,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -317,8 +326,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -633,8 +644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BADCF65-26F1-47F3-B466-D5B03A486648}">
   <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -690,10 +701,10 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>25</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>12</v>
@@ -747,19 +758,15 @@
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
-        <v>25</v>
-      </c>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="13"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{87F77614-4565-4D75-BA80-C984231769DA}"/>
+  </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -767,7 +774,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{934A0B2B-E659-44C6-A1CE-6954B3D336D3}">
   <dimension ref="A6:A7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -776,12 +783,12 @@
   <sheetData>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização e melhoramento do codigo
</commit_message>
<xml_diff>
--- a/src/main/java/br/com/rsinet/hub_tdd/cadastro/cadastro.xlsx
+++ b/src/main/java/br/com/rsinet/hub_tdd/cadastro/cadastro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rodrigo.vilhena\Documents\AvaliacaoTDD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61886C0F-1AB2-4C49-9615-062759360FB1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BF5DE1C-9FCB-4152-ABDE-9939012F14B6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="1" xr2:uid="{335E1E31-5428-4F3C-9976-AAC697D51952}"/>
   </bookViews>
@@ -112,10 +112,10 @@
     <t>Produto busca erro</t>
   </si>
   <si>
-    <t>Kingston Mouse</t>
-  </si>
-  <si>
     <t>mouse</t>
+  </si>
+  <si>
+    <t>KingstonMouse</t>
   </si>
 </sst>
 </file>
@@ -790,7 +790,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -809,10 +809,10 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
         <v>27</v>
-      </c>
-      <c r="B2" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refatoramento teste de cadastro
</commit_message>
<xml_diff>
--- a/src/main/java/br/com/rsinet/hub_tdd/cadastro/cadastro.xlsx
+++ b/src/main/java/br/com/rsinet/hub_tdd/cadastro/cadastro.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rodrigo.vilhena\Documents\AvaliacaoTDD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BF5DE1C-9FCB-4152-ABDE-9939012F14B6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C0B3C6F-C053-4B2B-93F0-1E0BE540158F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="1" xr2:uid="{335E1E31-5428-4F3C-9976-AAC697D51952}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{335E1E31-5428-4F3C-9976-AAC697D51952}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -82,12 +82,6 @@
     <t>Produto busca</t>
   </si>
   <si>
-    <t>RodrigoVil55</t>
-  </si>
-  <si>
-    <t>rodrigovilnateste@rstinet.com</t>
-  </si>
-  <si>
     <t>usuario</t>
   </si>
   <si>
@@ -116,6 +110,12 @@
   </si>
   <si>
     <t>KingstonMouse</t>
+  </si>
+  <si>
+    <t>bvilhena</t>
+  </si>
+  <si>
+    <t>rodrigovil@rstinet.com</t>
   </si>
 </sst>
 </file>
@@ -659,8 +659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BADCF65-26F1-47F3-B466-D5B03A486648}">
   <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -678,22 +678,22 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>20</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>22</v>
       </c>
       <c r="G1" s="8" t="s">
         <v>1</v>
@@ -705,21 +705,21 @@
         <v>3</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="K1" s="8" t="s">
         <v>4</v>
       </c>
       <c r="L1" s="9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="10" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>5</v>
@@ -789,7 +789,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{934A0B2B-E659-44C6-A1CE-6954B3D336D3}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -804,15 +804,15 @@
         <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Caso de busca de produto negativo - Sucesso
</commit_message>
<xml_diff>
--- a/src/main/java/br/com/rsinet/hub_tdd/cadastro/cadastro.xlsx
+++ b/src/main/java/br/com/rsinet/hub_tdd/cadastro/cadastro.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rodrigo.vilhena\Documents\AvaliacaoTDD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B92F6018-BBCA-4920-91F9-128456575409}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CFCFAEC-DBC0-4291-ABBF-4D4ADDD3B683}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{335E1E31-5428-4F3C-9976-AAC697D51952}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{335E1E31-5428-4F3C-9976-AAC697D51952}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -112,10 +112,10 @@
     <t>KingstonMouse</t>
   </si>
   <si>
-    <t>Braulioteste3</t>
-  </si>
-  <si>
-    <t>teste3@teste.com.br</t>
+    <t>Braulioteste4</t>
+  </si>
+  <si>
+    <t>teste4@teste.com.br</t>
   </si>
 </sst>
 </file>
@@ -669,7 +669,7 @@
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>